<commit_message>
Get daily reddit data: Tue Jan 21 08:10:38 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_26.xlsx
+++ b/data/collected_data/2025_01_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C503"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3440 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1i6dtd4</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>starting over 🥹</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6dtd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1i6dhdk</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>never used nail polish and have no desire to. (M)</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6dhdk/never_used_nail_polish_and_have_no_desire_to_m/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1i6d95c</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Looking for Polish Dupe Recs</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6d95c/looking_for_polish_dupe_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1i6cwb5</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Taupe’s neutral cat eye</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4vo898toaee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1i6c95b</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Latest set!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6c95b</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1i6c8va</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Snowy winter nails! ❄️</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6c8va</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1i6c7yf</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>L.A. colors ultra nail hardener</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6c7yf/la_colors_ultra_nail_hardener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1i6bfb3</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Short and dark...always look classic</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z668gb1o7aee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1i6bdz3</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails!!! </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd96dxpe7aee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1i6awbj</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Cat eye is so cool!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1lsorsv92aee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1i6ah3w</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shape recs for short nails on stubby fingers </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6ah3w/shape_recs_for_short_nails_on_stubby_fingers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1i69w29</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>I love them! Thanks to y’all’s help! 💜😍🩷</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i69w29</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1i69auz</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>I luv luv luv pink 🩷</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl2om90mm9ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1i68vr8</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Open to Criticism on Self Set</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f33ww91qi9ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1i68spp</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I chipped my nail. Is there anyway to fix it? </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkajm9syh9ee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1i68qjp</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Happy Face-Flame Stiletto Nails</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvikk0cfh9ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1i68lc6</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>where can i buy duck nail tips in store?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i68lc6/where_can_i_buy_duck_nail_tips_in_store/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1i68khc</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>BTArtBoxNails Press on Nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i68khc/btartboxnails_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1i681y0</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Does this cat eye set look right?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i681y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1i67y01</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>At home nails</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i67y01/at_home_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1i67pjx</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Nails smell like kitty litter?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i67pjx/nails_smell_like_kitty_litter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1i67et5</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdg8n8bh59ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1i66rd8</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Gorgeous green 💚</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i66rd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1i66nu9</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2nd try gel nails </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lql41kkty8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1i65xcr</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Why do my nails bend and snap in a half moon shape when they get long?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i65xcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1i6604j</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>My favorite nail set from last summer</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dli7460at8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1i65v3g</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun! </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ncdn534s8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1i65ta9</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Red will always be the best option for any occasion. ❤️</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1tgai2qr8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1i65k6c</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>This set was my last one of 2024, accompanied by beautiful jewelry. 🩵✨</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i65k6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1i65fay</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Nail dump</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i65fay</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1i62q6f</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Fractured nail?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i62q6f/fractured_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1i63okj</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chemical burn </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i63okj/chemical_burn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1i63syb</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Nails damaged after press ons</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i63syb</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1i65co1</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>In love with new set</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fj9o3vzn8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1i647nm</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Current set</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i647nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1i658a1</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>SNS nails chip? What do I ask for !?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i658a1/sns_nails_chip_what_do_i_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1i64u7u</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would you be OK with this manicure? How would you fix it? </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i64u7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1i65a3g</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gemstone Nails </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i65a3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1i6545q</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Weak nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6545q/weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1i64dy1</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>summer nails 🌊🩷🐚🏝️🌸</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xukbmvag8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1i63slr</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Do these look bad?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rxpcpukb8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1i63pwq</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>We continue with the beach mail theme</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i63pwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1i63mny</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Marble!!</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lue2e23ba8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1i6382n</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Love this set 💖</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyp75iz878ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1i636tx</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think it will be too much for many people, but I just love it. I love being creative and just having fun. I find art everywhere, be it in fashion, food or on my nails hehe. I hope you like it too :) </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3db3c7c68ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1i61y8m</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Acrygel Lifting</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i61y8m/acrygel_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1i61b1a</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>NSFW❗️❗️ Skin picking OCD</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i61b1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1i60wfn</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Nail change</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i60wfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1i60mf0</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Can’t go wrong!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn3vv2r7o7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1i60mcs</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did a set I'm really proud of but mt cuticles always look like they've gone through a paper shredder- any advice? </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i60mcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1i60gbv</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>They’re kinda cute</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oebj7eszm7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1i60de8</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>A little magnetic green with copper ^_^</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i60de8</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1i608xe</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Cant stop looking at my nails :)</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gyklqail7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1i605ia</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Dark mani for these dark January nights on natural nails</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i605ia</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1i5zzz5</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What am I doing wrong </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i5zzz5/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1i5zlka</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Structured manicure at home</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i5zlka/structured_manicure_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1i5yn0g</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips on how to get rid of nail breakage that starts in the nail? </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg77hlf2a7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1i5yohe</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>a nice manicure</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfho0beda7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1i5xzs3</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>new mani inspired by a post i saw here!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojnkjmrh57ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1i5y1pa</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Ryouma as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5y1pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1i5y16t</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Look at this set I just got done 😍</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5y16t</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1i5xqn0</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Not quite sure where I went wrong…</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i5xqn0/not_quite_sure_where_i_went_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1i5wu8k</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5wu8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1i5xkie</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Moon prism power 🌙✨💅🏽🩷</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnl5ixqh27ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1i5wqem</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Simple but beautiful💜</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zurqe3lw6ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1i5wm84</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>My manicurist is tired of me asking her for aurora powder but I can't stop. It's so cute</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9uqyqbrv6ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1i5w8ja</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🤍 </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5w8ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1i5vn9j</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set ♥️</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5vn9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1i5vj6a</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snoopy &amp; Woodstock Valentine’s! 🩷💌🫂 </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5vj6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1i5v6ii</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Xmas nail</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/542l4dmgl6ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1i5uzf3</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello Kitty Valentines Day Nails </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5uzf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1i5uv98</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>This is your sign to get your nails done to match your dog 💅</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5uv98</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1i5uojd</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>New year new pastel set💜💚🩵🩷</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5uojd</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1i5u56s</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ictgkitzd6ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1i5trzy</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>What color nails with this dress</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5trzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1i5tll6</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>ufo sighting</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5tll6</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1i5thxf</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Tips for skin picking</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5thxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1i5t80z</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>First builder gel overlay</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lta5by876ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1i5qg7o</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try at hand painted nails! </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnr09hatk5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1i5qenq</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Velaris / Night Court Inspired Nails 🌌💙✨</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5qenq</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1i5sli1</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>fav nude shade EVERRR</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awr9u8si26ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1i5rvtu</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>New manicure = good mood</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt7fy81vw5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1i5riu3</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Press ons for weak nails?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i5riu3/press_ons_for_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1i5r9xi</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Pink, pink everytime</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5r9xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1i5qwwb</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Valentine Nails</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5qwwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1i5qtw1</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to getting builder gel… is peeling normal? </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8aqdjlm4o5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1i5po3y</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did my own gel nails and now i have a green thing on my finger. Help please!! </t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3hk6ecad5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1i5p9yk</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkley pink </t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qurwpdy995ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1i5p5a3</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Is this shape ok for my hands?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5p5a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1i5ndn7</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Fluid nail art</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ealjfso3n4ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1i5lrwr</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Chocolate covered strawberry nails! 🍓🍫❤️</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5lrwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1i5llsr</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>How to make nails appear narrower</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i5llsr/how_to_make_nails_appear_narrower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1i6dnf2</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Anyone: how to make natural homemade nail polish?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6dnf2/anyone_how_to_make_natural_homemade_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1i6diq5</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>DIY cuticle oil success</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6diq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1i6cfad</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your favorite base coats that don’t have PVB? </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6cfad/what_are_your_favorite_base_coats_that_dont_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1i6c8bl</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>🕊️Mourning Dove, an eagerly awaited treasure 🥹</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6c8bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1i6be3r</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Love the look of magnetics, but they sure are time consuming 🥲</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4gn8vm3g7aee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1i6b9y0</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Dupe REQUEST!!!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6b9y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1i6aj37</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icy nails for south Texas icy weather. </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6aj37</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1i699ir</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>anyone want to refer me to cirque?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i699ir/anyone_want_to_refer_me_to_cirque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1i68d4z</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce </t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i68d4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1i685qf</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Purples 💜</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i685qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1i67fjv</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very demure, very mindful </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i67fjv/very_demure_very_mindful/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1i67fia</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Protect our Parks ⛰️ 🌳 ☀️ </t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i67fia</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1i672ay</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Update on Call Out Posts Rule + a guide how to post about customer experience</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i672ay/update_on_call_out_posts_rule_a_guide_how_to_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1i66qgn</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Gorgeous green 💚</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i66qgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1i66n5v</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>protest mani. queer inspiration. have pride, everyone.</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i66n5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1i66bf3</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Black for today. Pics before adding glitter</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkc4yg4xv8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1i65e0t</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Minimal nail polish collection</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77s814ly37ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1i65d5v</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Sparkling Aria</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i65d5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1i65c37</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Protest mani</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hx9tab2vn8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1i657n3</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zq1kb9jtm8ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1i6510z</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Found a steal at my local Walgreens!</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6510z</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1i64xhm</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Colors - Earthen.  Classic. </t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2iiij7lk8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1i63yqd</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scum and Villainy because, ya know, I’m just trying to get by </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i63yqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1i63rls</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>A shining moment in an otherwise gloomy day… 😻</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6fqy0ofab8ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1i63qdc</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>First stab at stamping with Zoya Tart &amp; Born Pretty White</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i63qdc/first_stab_at_stamping_with_zoya_tart_born_pretty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1i63aw0</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>🌈Rainbow Self Care🌈</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i63aw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1i63a6c</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>I always get distracted under the piano light when I’m wearing a holo 🤩</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i63a6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1i62u4q</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Royal purple 💜</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0qw1fde48ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1i62lm7</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>congrats</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mkex4koj28ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1i61rka</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about destashing </t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i61rka/question_about_destashing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1i6199z</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starry skies -makart blooming gel </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k8as6ors7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1i618un</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Couldn't decide what layer combo I liked better, so I went with a skittle!</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tjo22fcos7ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1i6153p</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Patrice by Zoya 💅✨</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0glqj6xr7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1i611mc</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At least my nails are ready for Sneauxmageddon </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fkrx519r7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1i603ua</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Charms from Walmart</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nu8uzahk7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1i5zsiy</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Starry Night🌌🌟</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5zsiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1i5ziqe</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>PSA: ILNP 30lb magnet</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ouy17obg7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1i5ypmm</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>fun holo moment!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5ypmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1i5yp4k</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>when ur mani is not quite the vibe but it's pretty anyway</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5yp4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1i5ymt7</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>What is this color?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5ymt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1i5ydb0</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Anyone else drawn to a brand because the bottles are so cute?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5ydb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1i5y46p</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Featured Guest for elephant toesies</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5y46p</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1i5xpi2</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>I love short nails</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgp4uqr437ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1i5xi8i</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Tracking my polish wear in my planner this year! Excited to see the trends unfold 💜</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqda54o127ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1i5xc4w</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>My wife pics my mani Part 4!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5xc4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1i5x3vp</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Dam GTFO My Uterus</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5x3vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1i5x0i0</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Show me your protest manis </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5x0i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1i5ww4a</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Snowin and glowin</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dd7dscb8v6ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1i5w8ji</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>I should paint my nails yellow more often 💛</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5w8ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1i5w2ow</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>The vibe today🦋✨❄️🫧</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q80h23zr6ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1i5w0ic</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Actually looks better in the shade :0</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5w0ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1i5vj6r</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Attempting Queen Beelzebub fluid art</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5vj6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1i5uzna</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>They're not sparkly! I'm lookin' for sparkles!</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1g9jn9uj6ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1i5uukw</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So much glow ✨️ </t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5uukw</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1i5ur6v</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to eat my chocolate nails </t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5ur6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1i5u65x</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>What strategies do you use to make the most of your collection?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5u65x/what_strategies_do_you_use_to_make_the_most_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1i5th93</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>mooncat 𖦹₊⊹ pomegranate seeds x demeter’s harvest ฅ^•ﻌ•^ฅ</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvc8daf396ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1i5tbmn</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Cracked Polish - “Leather Bound” - Appreciation!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5tbmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1i5t3xk</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>A very shifty purple combo 💜</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5t3xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1i5sw4m</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Petal pushers </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5sw4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1i5is9f</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Surprised by how much I love this jelly</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5is9f/surprised_by_how_much_i_love_this_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1i5s3q3</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Influenced</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5s3q3/influenced/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1i5sr2l</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Over buffed then over polished with gel</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5sr2l/over_buffed_then_over_polished_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1i5spgm</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Perfect winter shade🧊❄️🩵🤍</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uy1y1nla36ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1i5sgg7</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not into Star Wars but this polish is stunning!! </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z9oghnf816ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1i5se20</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Mooncat forbidden fruit: Fresh cat eye vs. 24h later</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5se20</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1i5s4m9</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Flower Child is seriously magical</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bqcj2axy5ee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1i5rwa1</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Simple periwinkle shimmer</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omlufyc5x5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1i5rn32</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>It's like having a personal sunset on your nails</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5rn32</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1i5q5sp</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Death Valley Nails thoughts on refracted light?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5q5sp/death_valley_nails_thoughts_on_refracted_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1i5q3tr</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Frosted</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/ZCK8Zb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1i5q1jp</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>The name matches the occasion, but the color is too fun</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdf7eq4yg5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1i5px09</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Disappointed how textured this is</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5px09</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1i5ptbd</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie pool party nails for summer 🏝️ </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5ptbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1i5pog3</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>What do I do about a tear this small? I’ve had my nails bare for almost 2 days oop</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi96gthdd5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1i5o3cz</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Seeking: Dupe of Mysteriously Me by Cracked Polish x Ethereal Lacquer collab</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5o3cz/seeking_dupe_of_mysteriously_me_by_cracked_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1i5nrog</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5nrog/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1i5noch</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>What are some good cheap international brands?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i5noch/what_are_some_good_cheap_international_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1i5n3zn</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Pipe dream</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5n3zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1i5m5t7</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Does anyone know what color this is?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37p3w22r64ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1i6cm63</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish + nail stickers. The purple glitter is very nice irl! </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6cm63</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1i6c8zt</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>L.A. colors ultra nail hardener</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i6c8zt/la_colors_ultra_nail_hardener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1i69se5</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Proposal is imminent and I can’t pick a design </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hy38ds0ar9ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1i66tnc</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>A little late, but I did a set for Wicked</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t4q4f8a09ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1i66fym</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>These have me feeling like a princess!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mg5kad0x8ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1i65am6</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gemstone Nails </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i65am6</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1i644ii</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">deep blue and light blue like a paradise island, I loved them </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i644ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1i63hqx</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Creepy But I Love Them</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i63hqx/creepy_but_i_love_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1i62ulv</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Glow in the dark rubber gel base set done by me :)</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i62ulv</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1i61i9l</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>junk journal inspired set</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i61i9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1i61g53</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Been doing nails for about a year</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i61g53</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1i60hgw</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>I painted my dog Murphy's cute little face on my thumbs and color-matched the rest of the nails to his hoodie (leg not pictured is a peachy color). Please be kind! :)</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i60hgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1i609jp</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>My Rustic Wood Nails!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5mkgeaml7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1i6037m</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Nail charms</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6037m</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1i5z22v</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Big Thumb Dragon for LNY</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5z22v</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1i5yoex</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Lunar New Year x Valentines Day</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/um5z3ozca7ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1i5y2fa</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Ryouma as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5y2fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1i5xylj</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Mushroom Forest Vibes (yes, the moon came out looking like the letter C)</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xb1zmu557ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1i5xkzb</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>New pink set 💖</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5xkzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1i5vpes</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set ♥️</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5vpes</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1i5u20t</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Fantastic, give me 14 of them right now 🥲</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3fc36scd6ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1i5s032</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Early Valentines Day nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cjogutyx5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1i5r740</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>D.va inspired nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ok3egl0cr5ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1i5r1t9</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some watercolor experimentation </t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5r1t9</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1i5pxa7</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>First time trying Gel x method</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5pxa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1i5olmg</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>first time doing proper nail art!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fgoqfct15ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1i5msp7</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails 🐍</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5msp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1i5mnvx</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">are they cute? </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i5mnvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1i5mfik</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Do you like it?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvutl4xha4ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1i5jx6a</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunflower Nails 🌻 </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb8xo2bjd3ee1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan 22 08:10:45 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_26.xlsx
+++ b/data/collected_data/2025_01_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C503"/>
+  <dimension ref="A1:C702"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8985,6 +8985,3389 @@
         </is>
       </c>
     </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1i76ceg</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>nails I did for my sister! she called them her raspberry lemonade nails</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i76ceg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1i75k3g</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Am i damaging my nails</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i75k3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1i74wrv</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>🪱🪲Hakuna Matata Nails 🐞🐛</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i74wrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1i74eat</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>February Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpaj3cu9ihee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1i740m2</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>New set❤️</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heglt131ehee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1i73xeg</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Suggestions for nail glue?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i73xeg/suggestions_for_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1i73ktk</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Because I'm basic and also... guess my favourite colour lol😂🤭</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i73ktk</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1i7335h</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>New nail shape</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bmul1cc4hee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1i731qs</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Just finished my first ever self-done dip powder set!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgpsh07y3hee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1i72fc2</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Matre gels</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i72fc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1i7209c</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Ideas ? Valentines nails</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3r49392gugee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1i71kj3</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I said “give me the goth Barbie look” and my tech delivered</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i71kj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1i71hme</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>What do you think? New to this 🥺</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mn178qj4qgee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1i71btt</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>The Icecream Set</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie0b1h8togee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1i7157u</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>There’s a cake on my finger!!! (V day set)</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7157u</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1i70vd2</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Any Tips?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j497p057lgee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1i70pk2</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Just some clean healthy newly-shortie nails</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i70pk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1i709ug</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>long vs short nails</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i709ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1i6zpj0</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Rubber base gel</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6zpj0/rubber_base_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1i6zx24</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Valentines Manicure! 🍒💌🎀</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6zx24</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1i6zmgu</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Nashly Nails? Brand Inquiry!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6zmgu/nashly_nails_brand_inquiry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1i6zf6m</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Does this look better.</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/untk4s9k8gee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1i6zbyl</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>After I stop biting my nails</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6zbyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1i6z3dl</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>First time doing my own nails!!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uku2ixeq5gee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1i6xd7t</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Nail salon etiquette</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6xd7t/nail_salon_etiquette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1i6yysm</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>My new way to be trans girl🥺rate Nail please and tips to start taking care of them.tanks ☺️</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvr8ih6n4gee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1i6yvk6</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Jewelry matching nails 🐍✨️</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6yvk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1i6ytsy</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>I promise to upload the last post about beach themed nails</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ytsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1i6ypui</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>My acrylic beads...aren't beads</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6ypui/my_acrylic_beadsarent_beads/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1i6y8xe</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Simpson Valentines Nail Set 🥰</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/piqyj7pkyfee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1i6y4d5</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Are these good?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6y4d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1i6y2o2</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>I rarely get my nails done but I decided to splurge. Short and simple.</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6y2o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1i6xs4h</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Nail health?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/red4fwxpufee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1i6xr02</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Sanrio Valentines Nails💗💗 freestyle I did the other day 😍</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wnfxmbhufee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1i6xbmq</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>First magnetic set!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6xbmq/first_magnetic_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1i6wi08</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>How to add charms??</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6wi08/how_to_add_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1i6we2u</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Instant Fail</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulatz7zhjfee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1i6w9ws</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>This effect is beautiful</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxnc7ttlifee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1i6voyy</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>First time using Kuromi X Apres Gel-X nail extension kit results</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6voyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1i6vhx2</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>First press on set. What do you think?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6vhx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1i6vhtk</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Edward scissorhands! 💅</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6vhtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1i6vbwa</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Beginner press on nails</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6vbwa/beginner_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1i6vb6s</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>First time trying Chrome</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vglsewa9bfee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1i6qb9d</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Both of my pinky nails are like this - does anyone know why? My other nail beds are totally normal.</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36d967siaeee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1i6um9d</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6um9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1i6ugsb</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>quick mani while baby naps</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ugsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1i6u4gi</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Health Anxiety with Nails</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxqwkmme2fee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1i6u36y</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Red wine feelings 🍷</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6u36y</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1i6tkjt</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Kiss press on nails</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6tkjt/kiss_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1i6ti7l</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Rainbow Mani</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ti7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1i6rfx0</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>crying in my room (vent)</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvz5pecsieee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1i6ta9r</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>It’s snowing in Texas.</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ta9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1i6t0h7</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Anyone else obsessed with French tips?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxmh6dbaueee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1i6stiu</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>First time using press-ons. Hoping they look okay</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vn7vpcluseee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1i6sn08</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>trying some color, I haven't decided if I like it lol</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6sn08</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1i6shnb</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>First tortoiseshell attempt!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dffwe3fqeee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1i6s66n</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>This set was my last one of 2024, accompanied by beautiful jewelry. 🩵✨</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6s66n</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1i6rifn</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>First time with acrylics-tips appreciated!</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6rifn</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1i6rgim</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>For the short nail girlies🦓🫧</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6rgim</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1i6qgpb</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My hobby favorite </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sxlhsvmbeee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1i6qeou</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>what do we think</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6qeou</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1i6pltg</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Fashion and nails 3</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6pltg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1i6pjca</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Best product to keep my cuticles looking fresh between mani/pedis?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6pjca/best_product_to_keep_my_cuticles_looking_fresh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1i6pawu</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Nosferatu nails 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6pawu</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1i6p4cy</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Getting length for wedding - dip with tips? Gel-X? What will last at the beach?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6p4cy/getting_length_for_wedding_dip_with_tips_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1i6oz95</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time!!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5vd18fw0eee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1i6okaq</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help please </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc6mitz0ydee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1i6oiud</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>What do you think? What type of nails do you think would suit my hands?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6oiud</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1i6lg1a</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Does anyone know why my nail started doing this?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqmpkeusadee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1i6nndo</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Been experimenting with gel glue and x coat press ons, how do you guys paint your own dominant hand?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6nndo</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1i6nvj8</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Thirty, flirty, somewhat thriving</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnfqkfj0tdee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1i6o3ur</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Holographic nails for the win</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obkw5gtpudee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1i6nhe2</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>My bday nails; garnet + year of the snake</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6nhe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1i6ndbk</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Some Nailfies</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ndbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1i6n6o1</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Red my favorite color for my nails</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vm7ppmxndee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1i6mtyq</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>What do you think ?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl2uvuz7ldee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1i6lnj7</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ateez inspired nails </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6lnj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1i6m0cc</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Girly pre-Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6m0cc</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1i6lkk1</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>What's the best nail glue for press-ons?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6lkk1/whats_the_best_nail_glue_for_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1i6lgfy</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please, need recommendations! </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6lgfy/please_need_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1i6l7a5</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombre cat-eye for this month's manicure. I'm in love with the subtlety. </t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygzs1iax8dee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1i6kaan</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Peeling skin around nails</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6n0f3bq1dee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1i6hbig</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I better off starting over? </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6hbig</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1i6ebwi</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Seeking advice from filthy casuals and seasoned pros.</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6ebwi/seeking_advice_from_filthy_casuals_and_seasoned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1i6dpgk</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Venting</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6dpgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1i6cif0</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Learning a new nail style uv lamp question </t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6cif0/learning_a_new_nail_style_uv_lamp_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1i6knwj</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Sistaco- How to remove?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6knwj/sistaco_how_to_remove/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1i6k34x</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Does this look okay?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6k34x</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1i6jvc0</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>nails, nails, nails</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6jvc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1i6jseq</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>My fifth set :3!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6jseq</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1i6jltx</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Everyone keeps complimenting my nails</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwat8zi1wcee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1i6jgbe</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’ve never really liked short nails but these are pretty :)) </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlrpziwqucee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1i6j851</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel-X I did on myself! </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6j851</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1i6j6a2</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Anyone knows how to lighten my cuticles and decrease wrinkles on my nails?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4j5912cscee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1i6ixdb</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Something extra💅🎀✨💗</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ixdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1i6iqrz</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Best press on nails from independent artists</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i6iqrz/best_press_on_nails_from_independent_artists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1i6i42w</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I usually get coffin with some nail art but decided to switch it up and go with something more classic 🖤</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6i42w</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1i6hznh</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite dopamine nails 🥰 💅 </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3j9oeul8hcee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1i6h9hg</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Mother of Pearls</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6h9hg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1i6gzuy</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Love my nail salon! Cheers</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6gzuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1i74wi4</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Another snowflake mani!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i74wi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1i74d9e</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Blackbird</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i74d9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1i74bx2</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Simple.</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hg1wwyjhhee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1i73zy4</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>When the kitchen lighting is 👌🏼 for linear holo</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i73zy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1i73v8k</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>I think I found my signature color 😍</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i73v8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1i73pjb</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Obsessed with these blue diamond nails for a snowy night ❄️</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i73pjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1i738wc</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Let's talk (daily) nail care! Cuticle oils, hand creams, and all the things!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i738wc/lets_talk_daily_nail_care_cuticle_oils_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1i734u7</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Talk me out of these? (Mooncat)</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rktu99ws4hee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1i730du</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Silvery</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxiaxm3l3hee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1i72vyx</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Rebelling against my winter swatch wheel</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i72vyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1i721lf</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Nail polish therapy is a very real thing.</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i721lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1i7181a</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>If you're new to painting your nails, do yourself a favor and buy a quick dry top coat immediately!</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7181a/if_youre_new_to_painting_your_nails_do_yourself_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1i70rfa</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Favorite gel base/top coats?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i70rfa/favorite_gel_basetop_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1i708u7</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Painted my nails 9 hours ago and just got these imprints :( any advice?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i708u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1i6zs8x</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>A better linear holo topper than Holo Taco’s?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6zs8x/a_better_linear_holo_topper_than_holo_tacos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1i6ze5x</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Taking a break from press on nails. What should I use? *please read description!* REPOST FOR ADDED INFO</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ze5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1i6z90i</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Dupe for this polish??</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99vob3637gee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1i6z1dw</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>INM Out The Door dries wrinkly?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p58yw55a5gee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1i6z19m</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Usually not a purple gal but I can't get over this alexandrite!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y7dn3z995gee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1i6z186</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>First textured polish</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6z186</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1i6yzrw</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Deep Space is everything they say</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka05v25v4gee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1i6ycb5</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>like candy on my nails 🤩</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8g86gzdzfee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1i6ycan</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>is he everything you fear!!!!! 👻👻</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcr0b8zdzfee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1i6xvrh</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Nonbinary skittle</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nb0a820lvfee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1i6xehd</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Regular Magnetic Mani</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lhj03seqrfee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1i6x66z</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Taking a break from press on nails. What should I use? *please read description!*</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k70yaniupfee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1i6x3nf</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>ILNP Evermore</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzv7axt9pfee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1i6wubu</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Valentine’s jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6wubu</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1i6wk20</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>nail youtube?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6wk20/nail_youtube/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1i6wgqd</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Snow day in Louisiana!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6wgqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1i6wa25</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>The most iconic lacquers?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6wa25/the_most_iconic_lacquers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1i6v4el</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>How to stop thumb nails splitting</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6v4el/how_to_stop_thumb_nails_splitting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1i6ty9r</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>On the hunt for green/purple multichromes/shimmers</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6ty9r/on_the_hunt_for_greenpurple_multichromesshimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1i6trb0</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Anyone know what might be happening when nail polish takes too long to dry?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6trb0/anyone_know_what_might_be_happening_when_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1i6tkvi</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Rainbow Mani</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6tkvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1i6tjp4</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>i really like this coppery orange 💅</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6tjp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1i6tgt7</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Tracking 2025 Manicures with Swatches</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu0s2ickxeee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1i6t0pm</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>In love is an understatement</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/13irdn3aueee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1i6st3u</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>baby’s first (and only) thermal! i loveeee this color 🌌💙💚</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6st3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1i6sf95</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>ILNP Enchantment after 4 days</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6wd3gepxpeee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1i6s4r8</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Pretty polish as a ✨distraction✨</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6s4r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1i6rl6a</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>I need to practice my layering</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kucy54ujeee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1i6rgzz</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t xml:space="preserve">January blues 💙 </t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6r7c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1i6r9eo</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Velvet nails</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/082ciqvgheee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1i6r7oq</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>What would you do...?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6r7oq/what_would_you_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1i6r1c6</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Keeping track in 2025</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdccd4iufeee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1i6q8i2</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Contender for polish of the month</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9er4yzk0aeee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1i6pz6q</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Has anyone else been having bad nail polish days? 😭</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6pz6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1i6py80</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Dark Skittle</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wmt1zly7eee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1i6pgt5</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Thistle and Thorn</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6pgt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1i6pe7p</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>What are some polishes that nail a reference or create an image in your head?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6pe7p/what_are_some_polishes_that_nail_a_reference_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1i6ozbd</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Kaleidoscope my first Baroness X polish</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ozbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1i6otrv</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rubber base gel or Builder gel under polish? </t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6otrv/rubber_base_gel_or_builder_gel_under_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1i6os98</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Cock-A-Doodle-Doom is everything I hoped for!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvgm0nthzdee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1i6o7ij</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>First lobsters, now snakes 🐍: shade match recommendation for this rainbow python?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6o7ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1i6o1q0</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>ILNP VIP</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/33jjn6t9udee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1i6nn6x</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there a way to create this effect with regular polish? </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbpkbf7crdee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1i6ncx1</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chameleon Coat - for everyone who needs to blend to feel safe </t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ncx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1i6ncqq</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deep reds (oxblood, burgundy, etc) have sorta become my comfort color in the last couple months. Dark colors look good on short nails &amp; I have to cut my nails down completely every couple weeks because I’m anemic and despite taking iron supplements, they peel / break so easily now 😞 </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ncqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1i6n872</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails to see Nosferatu today! (Finally) </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6n872</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1i6mvgb</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Mooncat's Jewel Beetle lives up to its name</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1v5ym9qkldee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1i6mnat</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Starting somewhere</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6mnat</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1i6may6</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Death Star-stroyer</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6may6</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1i6lk8g</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>🩷🌵Cheyenne🐄🩷</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6lk8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1i6lazu</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Is it hard to believe I used two different oranges on each nail? lol</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6lazu</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1i6kime</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Eternal glow</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6kime/eternal_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1i6kfsa</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>An homage to Moolissa 🐮</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6kfsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1i6iuu8</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Cirque’s Blue Velvet</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y5gx6mvfpcee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1i6bk38</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question About Half Broken Gel Nail and Preventing Contact Dermatitis </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i6bk38/question_about_half_broken_gel_nail_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1i6fpgb</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>First Nail Art + builder gel question</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t14si11rbee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1i6i5m6</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Mememto Mori is to DIE for (pun intended)</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6i5m6</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1i6hidz</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk2qpwnfccee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1i75d64</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Starting my resistance set lol</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rd45ny3vthee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1i752tl</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>A bit of growth</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i752tl</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1i750hd</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Howls Bedroom</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zp2r46hphee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1i74zw6</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Trying out some new brushes I got</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8qeggkaphee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1i71ooi</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Just started my stamping journey!!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i71ooi</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1i70xtd</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>3D nail art</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tzbt0oqlgee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1i70q3p</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Pink and Green press ons!</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iztrsdi1kgee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1i6zpot</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Picnic nails</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6zpot</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1i6ywtn</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Best starters practice kit</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i6ywtn/best_starters_practice_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1i6yllu</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Acrylic powder mixed with gel. 3D art. Yay or Nay.</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6yllu</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1i6y8ev</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Simpson Valentines Nail Set 🥰</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi9g0zegyfee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1i6tuy8</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Tropical vacation nails🌺</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6tuy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1i6tt56</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Feedback on my mom's nail extension work</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6tt56</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1i6tmnq</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Xmas press ons I made for my mum (red) and I (white base)</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6tmnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1i6qgbh</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Stained glass nails 🙂</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6qgbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1i6piw1</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Fashion and nails 3</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6piw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1i6p13b</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Space Vibes</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6p13b</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1i6onn9</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Bday nails; garnet + year of the snake</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6onn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1i6ondz</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Tips for spider gell</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ondz</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1i6kt0i</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Eyeshadow keeps wiping off on gel nail/ top layer doesn't apply properly</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6kt0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1i6k6wf</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails art for men </t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6k6wf</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1i6ihg2</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red and gold  </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea9p96bzlcee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1i6hm7u</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whimsical nails 🧚‍♀️✨ Gel x on natural nails </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6hm7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1i6ghqp</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time making press on nails </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6ghqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1i6fx83</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>There's no such a thing like too much sparkle 💖</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7qtaqkutbee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1i6frt2</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a little bit of frost </t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ond8zwturbee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1i6fa3p</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherries </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i6fa3p</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan 23 08:11:03 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_26.xlsx
+++ b/data/collected_data/2025_01_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C702"/>
+  <dimension ref="A1:C909"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12368,6 +12368,3525 @@
         </is>
       </c>
     </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1i7vz3i</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>My engagement is in two days…</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7vz3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1i7xzz3</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Late post for Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7xzz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1i7yhfv</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Is there a gel polish that matches this?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njeobtjm9pee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1i7y5zt</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Did my nail tech do a good job of shaping?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7y5zt</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1i7xpya</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>January set</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9r942b7zoee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1i7vy5d</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Nude Colour Advice</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4z68zbaeoee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1i7x00p</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I remade my ghostbusters nails on some press ons for my birthday and I love them!</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7x00p</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1i7wumb</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7wumb/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1i7wtke</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>All of my nails since March of last year</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7wtke</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1i7wmw1</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Tried out a magnetic glitter for the first time &amp; I can’t stop staring at them 🥹✨</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/otv3eub1moee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1i7wjl0</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Last Set | Current Set</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7wjl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1i7w9b5</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Am I crazy or did my nail tech do a poor job with the shape</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7w9b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1i7w6zy</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Polygel vs acrylic?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7w6zy/polygel_vs_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1i7w18q</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Valentine’s day ❤️</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzdjxt18foee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1i7vnse</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Someone Pls tell me what color/ nailpaint this is?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7zc0fn9boee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1i7vhum</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>These are so fun and cute!!!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t87m8eqj9oee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1i7va44</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>How can I improve my nail shape? There are so many choices for shapes and I’m a little lost what direction to go. Any advice appreciated.</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7va44</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1i7ur9j</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>White on white frenchies 🥛</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrw994m72oee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1i7ukk0</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Blue and black Goth nails</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhmi9cbd0oee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1i7uata</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Short, bendy nails.</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7uata/short_bendy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1i7u0ci</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Valentines but make them extra</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi3oypr2vnee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1i7ty0t</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>My natural nails 🤍</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7ty0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1i7tvtn</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Smooth nails, pink tones with embossed gold details</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7tvtn</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1i7tuwx</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>It’s giving Gothic Cathedral 🩸🦇🗡️</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mzgg48ptnee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1i7ssgl</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Fallout Inspired</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7ssgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1i7tema</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>This may be a stupid post..</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adybewdmpnee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1i7swt1</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Watercolor with gel polish</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7swt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1i7slrm</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>I recently got into nail art and theses are the sets i've done since christmas (in order from oldest to newest)</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7slrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1i7slf6</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>First time trying press-on nails!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7slf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1i7npk6</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Bump in nail after reaction</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7npk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1i7q4bp</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Help!! What to ask for?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7q4bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1i7qfiy</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Gel peeling or corners lifting</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzngnzqqzmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1i7qjxq</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Nails that Last a Day or Two?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7qjxq/nails_that_last_a_day_or_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1i7rhm4</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Someone please tell me it’s not a big deal…</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7rhm4/someone_please_tell_me_its_not_a_big_deal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1i7qurd</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>I'm practicing painting portraits 🫠 7 hours in with a new technique and my WRISTS ARE ACHING 😭</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag3cxfb93nee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1i7r86b</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>My nails today! What you think?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6gmf90g6nee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1i7r699</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>who loves this color ?????</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/deuf7w8z5nee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1i7r61n</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>how to make gel nails look better?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7r61n/how_to_make_gel_nails_look_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1i7qkbq</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Freestyle for CNY 🧧</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aopg8qtu0nee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1i7pu3u</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>What type of manicure (that is fairly chip resistant) is your favorite?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7pu3u/what_type_of_manicure_that_is_fairly_chip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1i7psh3</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>I’ve tried everything and my nails won’t grow past my fingertips - what else can I try?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7psh3/ive_tried_everything_and_my_nails_wont_grow_past/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1i7pgch</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Swirls🌀</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dol78rwrmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1i7pdke</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>I love butterflies</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1271to9rmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1i7p68x</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Latest set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2vusadmpmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1i7p1d7</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>My latest set 🖤</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl6k182jomee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1i7ozqh</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Question about acrylics</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7ozqh/question_about_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1i7ow65</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Willing test subject number 2</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx905o6dnmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1i7o9op</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Starry nails 🌟✨💫</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7o9op</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1i7o9ju</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Icy Lilac</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7i6djhjjimee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1i7o7r6</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Iridescent Nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cna83p25imee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1i7o5kl</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>I found my nail person 🥹</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sa8qfasohmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1i7o4p9</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Ombre cat eye 💅</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guwz8ohihmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1i7o2kw</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Helps</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi8xaff2hmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1i7nl0s</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Final no extensions! My full nail length! Sanrio Little Twin Star inspired</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ut34f50ddmee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1i7n7k2</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Obsessed with cat eye lately 🌌</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1abkqsmamee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1i7mq95</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Finally got my nails done after months without 💅🏽</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktu3w1nz6mee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1i7mgtz</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Is this still wintery?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/521eq3115mee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1i7meex</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>my nails are horribly thin but ive successfully grown them out !</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7meex</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1i7lmz2</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Vintage Gel X Nails</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7lmz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1i7lllm</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Yay or nay on short acrylics?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7lllm</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1i7lf0y</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>V-Day nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7lf0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1i7kui6</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Menchie the Cat never fails to brighten my day 🥰</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7kui6</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1i7kbx8</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>New day new nails I just love doing my nails. And yes I also have diamonds on my steering wheel hehe I just love it and I think it will be too much for most people</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3n1a0o6qolee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1i7kaij</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>valentine's 2025</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7kaij</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1i7k0k3</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set 💗</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uqfmc0zmlee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1i7juwt</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Work a manual job and can't seem to get dead skin off the sides of the nail beds</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oki9drbtllee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1i7frqy</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>dark blue jelly nails for a freezing january. 🥶</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/duwmzjcuskee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1i7jgty</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>My nails “aurora effect” 💖</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcj18yt3jlee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1i7jbbb</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7jbbb/wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1i7jb29</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Someone validate me for having $30 nail polish even though I never paint my nails. Golf le fleur by Tyler, the creator. This is the best polish job I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7jb29</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1i7j5d8</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Best nail shape for my hand?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7j5d8/best_nail_shape_for_my_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1i7iswf</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Feeling shifty</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tta0i1rhelee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1i7iij3</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Gel lifting!?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7iij3</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1i7ib9m</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Tutorial for how I remove nail glue from my skin</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hw1npcm0blee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1i7hg7s</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Severely damaged, thin nails--need advice on whether a hard gel base with short extensions is right for me and if so, what overlay would be best!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7hg7s/severely_damaged_thin_nailsneed_advice_on_whether/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1i7heau</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Chain Legend - King of Hearts ❤️</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7heau</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1i7h7o8</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>First professional manicure, SO obsessed</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1gw7lq73lee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1i7g7vl</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>First time giving myself a gel mani! Used the Olive and June gel system. Please give me your recommendations for daily cuticle oils☺️</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7g7vl</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1i7g6ww</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Nail tech removed acrylics by cutting and ripping them off ?!</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7g6ww/nail_tech_removed_acrylics_by_cutting_and_ripping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1i7g5xi</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>First time trying mooncat polish. Tried both hands and toesies! (Color: Not Today Satan)</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rj95u9ojvkee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1i7g1tu</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Polish for kids that won't peel off right away?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7g1tu/polish_for_kids_that_wont_peel_off_right_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1i7fv5a</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Obsessed 🥀🍒🩸</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7fv5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1i7fsnt</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>perfect for the season 🩵💕❤️</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eslg03n0tkee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1i7fqtg</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Clionadh - Acid Rain</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13kqf4cnskee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1i7f3ti</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Onycholysis (help and advice)</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7f3ti/onycholysis_help_and_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1i7esc3</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>MAGNETIC CAT EYE NAILS</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7esc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1i7eqy7</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Things I learned from this sub!!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7eqy7/things_i_learned_from_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1i7bkdw</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Sally Hansen Insta Dri with Matte top (same brand) and essence Glazed Donut top</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myy7vw21wjee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1i7dgj6</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Pink vs Pink (Clean Girl Cateye?)</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7dgj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1i7dtrs</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Which is easier at home method?/ questions about UV/LED lamps</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7dtrs/which_is_easier_at_home_method_questions_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1i7bpum</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Did my nail beds actually get bigger??</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7bpum</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1i7d0o8</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Builder Gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7d0o8/builder_gel_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1i7cv7c</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Thank you everyone for your advice on my cuticles! They're looking a lot better</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3059rud07kee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1i7cszw</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Rainbow press ons!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7cszw</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1i7c4a4</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Best glue/gel?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i7c4a4/best_gluegel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1i7b91z</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>First time I’ve done my own acrylics!! Thoughts and tips please 🙏</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7b91z</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1i7ay8u</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Nutty nougat neutral</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7ay8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1i7apmz</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Not so ready for valentines nail 😆</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo154mg2ojee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1i7ade4</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>nude 🤍</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49j4w1gskjee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1i792kf</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I love getting black nails, when all are glossy except for one with matte finish 🥰</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i792kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1i7xk72</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Cirque Colors really cannot take any constructive criticism and I'm done with them.</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7xk72/cirque_colors_really_cannot_take_any_constructive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1i7x3w5</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Transform dupe help</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7x3w5/dazzle_dry_transform_dupe_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1i7x0se</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Anyone bought from Voyage Hues before?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wpcye7kqoee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1i7wyyc</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>help 🥲</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrrjkirxpoee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1i7wfdb</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Intuition&gt;Overthinking</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7wfdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1i7w2ws</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Any suggestions for similar dark fuschia/berry shades like in this picture?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7w2ws/any_suggestions_for_similar_dark_fuschiaberry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1i7v4kj</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Cirque Juicy Fruit</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7v4kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1i7v3c2</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Sassy Sauce never misses</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7v3c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1i7uis4</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>A Feverish Orphan With A Soup Deficiency</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7uis4</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1i7ufna</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zl7xmf72znee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1i7ua24</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Fancy Gloss-Queen Bee</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwh23w8kxnee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1i7u99m</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>What polishes do you prefer one coat of?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7u99m/what_polishes_do_you_prefer_one_coat_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1i7tyo6</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>what can i do to improve longevity?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7tyo6/what_can_i_do_to_improve_longevity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1i7twv6</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>First time painting: Split Decision Nails 😂</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yduybs73unee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1i7tx0t</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>it’s  ✨Our✨  season now  ♒️ Happy birthday Queens</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7tx0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1i7tvqw</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>ISO Pure Ice - First Love dupe!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://gingerlypolished.com/2016/10/23/swatch-my-stash-pure-ice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1i7ts3i</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Looking for swatch of Lumen - Silver Fox</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7ts3i/looking_for_swatch_of_lumen_silver_fox/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1i7sncz</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Can someone explain silk wraps to me?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7sncz/can_someone_explain_silk_wraps_to_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1i7sf0h</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Looking for grape purple polishes like the one pictured</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl7z0jmpgnee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1i7s84s</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for these two shades</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g9xrv02fnee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1i7rwb1</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzpm8e77cnee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1i7rg3c</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Trippy Dippy Psychedelic Mushrooms - By Kate @Tropical Popical on me</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ugzknrz7nee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1i7rf5q</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>I need to order Thinner. Never ordered from kb shimmer before. Opinions?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gpucgm18nee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1i7qsh4</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>fairy nails in the snow</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7qsh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1i7qobh</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Glowing opal mermaid snow princess! ❄️</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7qobh</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1i7qkyr</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer-Judgement</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7qkyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1i7qfqt</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>My (accidental) Wicked mani! 💚🩷 I love this polish topper with nudes and pinks so I decided to try it with a darker color and it resulted in a perfect Wicked inspired mani! 😂</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7qfqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1i7qcbr</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Mooncat catfished + star destroyer</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7qcbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1i7qbf6</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Non Gel Jelly nail polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>/r/Nails/comments/pdezzt/non_gel_jelly_nail_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1i7fyov</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>4 coats of essie limo-scene, kiss halloween stickers, 1-2 coats of seche vite</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7fyov</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1i7lbkr</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Looking for a lacquer like this</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7lbkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1i7mdw0</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Recent manis</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7mdw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1i7q138</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Using polish thinner on quick dry top coat</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7q138/using_polish_thinner_on_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1i7pm00</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>California Love (Cracked charity polish)</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7pm00</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1i7oyvs</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>✨ Clionadh Cosmetics 6 new Slick-adelic Magnetics + opening the vault!</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/DFEhlJzNC4L/?hl=en&amp;img_index=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1i7oxyh</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Zoya Josie and Zoya Ness: the same color?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csnorx3rnmee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1i7os0p</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Sally Hansen Insta-Dri Syrup Jellies</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7os0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1i7o9tj</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Mermaid Scales 🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7o9tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1i7o8fv</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>birthday mani</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfanpp0bimee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1i7nvdh</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I've never gotten so many compliments on my nails before!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7nvdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1i7ns4e</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Is it normal to have cuticles bleeding after dip manicures?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7ns4e/is_it_normal_to_have_cuticles_bleeding_after_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1i7nhsw</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>when you get one tiny chip in your nail and it’s all you see 🙂</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7nhsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1i7nbqi</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Here's my lacquer therapy</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7nbqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1i7n3ye</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Baby Blue Recommendation</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7n3ye/baby_blue_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1i7mr4g</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>I've been waiting since Christmas for this...</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7mr4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1i7mqo2</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Anyone know a dupe of my favorite old ‘live love polish’ polish?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkpo8uu27mee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1i7li53</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>First Polished For Days order!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r17dtjwpxlee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1i7kqgp</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Arctic Confetti</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7kqgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1i7k4lb</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Clionadh Canada shipping?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7k4lb/clionadh_canada_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1i7jq1i</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>what happened to this polish? sold-out or discontinued because i can’t find it on the mooncat website 😭</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wstz67lwklee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1i7jm1j</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Is anyone else trying reverse velvet?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7jm1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1i7jaqu</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Walmart/Target Suggestions for College Student?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7jaqu/walmarttarget_suggestions_for_college_student/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1i7ixcl</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer- Choose Life</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ar053ghbflee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1i7ixbr</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Clionadh Swatches?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7ixbr/clionadh_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1i7iuth</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>New Favorite Polishes</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7iuth</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1i7ine2</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Photo Tips?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7ine2/photo_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1i7ilnk</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>eternal glow 🌟</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7ilnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1i7iies</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>These look even better than I imagined</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bs0bpaifclee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1i7hq1q</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Winter ombre</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/beovxe1u6lee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1i7hgt4</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>ILNP Newbie - what do y'all love and what do y'all hate?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7hgt4/ilnp_newbie_what_do_yall_love_and_what_do_yall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1i7hbom</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Emily de Molly - A Veiled Promise</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p2lvi1n14lee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1i7h8ot</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Another chrome on regular polish success!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7h8ot</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1i7gikk</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Enchanted to meet you</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7gikk</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1i7gi4c</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>florida snow day nails ☃️</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7gi4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1i7gbk9</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>❄️🐚 Snow at the beach…</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1wxfzamnwkee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1i7fxdl</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Mooncat dupe?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7fxdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1i7fr3p</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics- Acid Rain</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5s7x6lpskee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1i7fmja</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Is there a Holo Taco/ILNP dupe for this?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4p5znkirrkee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1i7fl43</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Zoya Autumn is that girl</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7fl43</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1i7eofw</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Brown, Gray, Green Swatches</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0hqcrhrkkee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1i7en1b</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Seeking dupes and a question on brown polish</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7en1b/seeking_dupes_and_a_question_on_brown_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1i7edo6</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Wanted to do some kind of protest nail art and settled on this design. Simple but effective.</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7edo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1i7e2sp</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Dusty/muave pink magnetics</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7e2sp/dustymuave_pink_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1i7druz</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Rose Quartz Nails</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7druz</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1i7d2x6</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Orly Neon Swatches</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7d2x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1i7cz4t</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Cirque Dioptase</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7cz4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1i7cvpg</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Mooncat’s Dearly Departing</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5le43r47kee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1i7cqhu</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I'm about to make my first ILNP purchase!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7cqhu/im_about_to_make_my_first_ilnp_purchase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1i7cnwr</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>When you accidentally match your nails to your Nalgene...</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjndm56c5kee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1i7cm4d</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Flakies and sparkles to boost mood</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy174arw4kee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1i7cg60</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Is there a ridge filler that doesn’t take forever to dry?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7cg60/is_there_a_ridge_filler_that_doesnt_take_forever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1i7btkc</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Some Pokémon nails I did with stickers from Etsy!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7btkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1i79c5s</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Skye is the limit</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i79c5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1i793zs</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Essie - Semi-precious tones</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88t3hfn87jee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1i78k44</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>French Nails - base too peachy</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meushr1l0jee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1i781on</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Park Ave</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kotd1v1ttiee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1i76pzc</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Any tips for beginner at painting nails?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i76pzc/any_tips_for_beginner_at_painting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1i7xrwt</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Best way to practice?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i7xrwt/best_way_to_practice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1i7uoj5</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>I loved making this set</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/re1tzt0h1oee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1i7tk5b</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>No me gusta tanto el color blanco pero quedó bonito.</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0vaz9g0rnee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1i7seu7</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Mimikyu inspired nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1mmwa4ognee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1i7rpsi</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>first attempt at character nail art</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7rpsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1i7qv4o</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>I'm practicing painting portraits 🫠 7 hours in with a new technique and my WRISTS ARE ACHING 😭</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opaqosxc3nee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1i7kgi2</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Random Set</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5kck0k4qlee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1i7jenn</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>nail charms chipping even with top coat?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dmzstxoilee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1i7iglk</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Valentine freestyle</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7iglk</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1i7hu2r</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Made these for my girlfriend</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7hu2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1i7h2hi</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>I'm going to graduate and I did these nails! If only they matched the red wine dress?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/okkqolx02lee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1i7dh8i</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>What do you think of my nails?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l07w15wsbkee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1i7gp3d</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Recreation of an old nail set</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7gp3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1i7fbnb</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>6th set I’ve done on myself</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0rokb5jpkee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1i7f7q9</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Spot which one was the first one attempted 😅</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qpm1l3rokee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1i7d817</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>happy because the ribbon turned out nice</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7d817</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1i7cohf</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Is this a recent trend? I was inspired by something I saw recently. If it is, what is it called?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gv2ho6rg5kee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1i7cm0x</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Tortoise Shell 🐢🤎✨</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7cm0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1i78s8u</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i78s8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1i6zlxd</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>How about this design for Valentine's Day?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om7agem8agee1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan 24 08:10:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_26.xlsx
+++ b/data/collected_data/2025_01_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C909"/>
+  <dimension ref="A1:C1098"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15887,6 +15887,3219 @@
         </is>
       </c>
     </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1i8q5gi</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Who else loves reading when they have their nails done??</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz0q20ly9wee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1i8pp3n</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>I love them simple yet classy 💅🏼</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8pp3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1i8pjy3</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Valentines ready</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/thunderousfirmzebrafish</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1i8nf77</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Icy ombre 🩵🌨️❄️⛸️🧊</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8nf77</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1i8ozzg</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>First set of 2025!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8ozzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1i8pdip</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Nail tech put on gel-x crooked…do I try to file and fix myself or go back?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8pdip</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1i8p6xf</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Are my nail beds long or short?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8p6xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1i8p188</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>I count these as early Vday nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpwsamdxvvee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1i8oigw</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Need help getting nail drill gift!!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8oigw/need_help_getting_nail_drill_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1i8o92s</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>olive &amp; june press-ons????</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8o92s/olive_june_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1i8nym1</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>How avoid pooling in cuticle?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8nym1/how_avoid_pooling_in_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1i8ntqy</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>🧁</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2feozzzmivee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1i8nkve</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Fluid Nail Art Attempt #2</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8nkve</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1i8nhev</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Just made a set for CNY 🐍💖 thoughts?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8nhev</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1i8n526</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Give me VALENTINES IDEAS!</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8n526/give_me_valentines_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1i8lojz</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Cuticles in need some serious TLC. Please HELPPP</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gif15ptgxuee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1i8lv62</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>What do I need to start doing my wife’s nails ?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8lv62/what_do_i_need_to_start_doing_my_wifes_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1i8moa3</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>first time getting gel x :)</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8moa3</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1i8mcff</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>accidentally matched with a carrot</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tum9ulto3vee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1i8m3m9</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>apex check–too flat?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8m3m9</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1i8m0hq</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Late post - New Year’s nails 🎆</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8m0hq</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1i8lwn5</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>A little prettier</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bxc5o7fzuee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1i8lkv2</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>this set is beautiful</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxjiz21jwuee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1i8kyss</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I'm in love</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8kyss</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1i8kxpm</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Basic question</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8kxpm/basic_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1i8kgc8</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Returned from getting my nails done with a stomachache.</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8kgc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1i8kf9d</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>SpongeBob!I think I did pretty well</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4ii5hz3muee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1i8k5u7</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Tried almond for the first time 😍</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8k5u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1i8jytr</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Nails are stained, any tips?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8jytr/nails_are_stained_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1i8jdlb</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Takumi as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8jdlb</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1i8itr7</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Genuinely proud of these :)</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8itr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1i8gfnl</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>does anyone else experience pain when getting nails done?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8gfnl/does_anyone_else_experience_pain_when_getting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1i8hij6</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Manicurist - does it work?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8hij6/manicurist_does_it_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1i8iodz</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Finished painting BBNO$ on his practice nail with the new technique and top coat 😭</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6xsh7nt6uee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1i8igcw</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>All the nails I’ve done in my first week of making press ons 💖🥹</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8igcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1i8iejt</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>One week after getting acrylic fill</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvmlcosj4uee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1i8i4dp</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>setting the tone for a gloomy January</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8i4dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1i8h7gi</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Finally got my nails done again after almost 2 years! My nail tech, Jocelyn, always does an amazing job 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8h7gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1i8h6ip</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>birthday nails!!!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jeelcbvgutee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1i8h3tl</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Red chrome</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2omirovttee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1i8h0ba</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>My first time trying 3d nail art gel ( candy carving gel )</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8h0ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1i8g58n</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Love these that my girl knocked out!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9kp8na6mtee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1i8g3ne</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>WIP press ons for my first client ☺️</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8ro5s1ultee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1i8ffuo</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Valentine’s nails 💝</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8ffuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1i8fa26</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>In LOVE 🖤🖤</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8fa26</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1i8f9rg</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Here’s my nails. Does anyone else love glue on nails?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxz3u9fjftee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1i8exrh</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Is there any way to fix this? It makes shaping my nails (having consistent nail shape throughout my hands) very difficult!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8exrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1i8eefy</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/le6xi95y8tee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1i8e8nh</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>First attempt🧊What do you think?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze0rgnvq7tee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1i8e7ni</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>New year, new nails</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8e7ni</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1i8dvn8</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Cat eye birthday nails 🩵🤍</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jn8c5f55tee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1i8dq3z</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Searching for a builder</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8dq3z/searching_for_a_builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1i8dpda</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Beginner Tech Prices</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8dpda</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1i8dp38</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Most recent set 🎀</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iezgsshs3tee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1i8dabj</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>just wanted to share the set i did yesterday.</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db4v6m8r0tee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1i8d0yx</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>hey guys! i have a job that doesn’t allow nails to be painted, is there some kind of reusable press on brand that’s good?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8d0yx/hey_guys_i_have_a_job_that_doesnt_allow_nails_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1i8c75p</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Does anyone use low odour monomer?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8c75p/does_anyone_use_low_odour_monomer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1i8bmns</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Current set</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dofl3at9osee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1i8bmkv</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Gravity falls!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhubw20cosee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1i8bd77</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>My birthday nails</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8bd77</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1i8aqp1</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>My first nail set with charms 💕</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8aqp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1i8ajr9</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Kitty nails! 😻</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8ajr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1i8aba1</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Basic but pretty ✨</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8aba1</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1i8a8zm</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Can't Believe It Took Me So Long to Join!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f9tn91lcesee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1i8a6rm</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>I've already scratched myself</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vf72uqrxdsee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1i8a10u</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Help! Please suggest nail polish color</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/behs8eorcsee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1i89qvs</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Pink Glitter Nails</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mwcf99qasee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1i89lp9</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Picture of my natural nails before cutting them, before they become dangerous for myself. 🥹</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i89lp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1i89kd4</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>One of my favs 🌸</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dysglye9see1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1i88vxo</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>We called this one princess unicorn 🦄👑</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i88vxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1i88tg0</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>do you like it?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dbb8ccv3see1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1i88nph</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Dip, Gel or GelX. Which is the best?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i88nph/dip_gel_or_gelx_which_is_the_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1i882d2</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>New set and cuticles fully healed. I just e-filed down the set I had before as they were too bulky and then a cat eye with a rose jelly polish over the top</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yalyl51gyree1</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1i87wfz</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>How do we feel about these? I’m obsessed #freehand</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfdx3898xree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1i87i2m</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>question about builder gel vs bio gel</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i87i2m/question_about_builder_gel_vs_bio_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1i86p2h</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Oval or square for me ?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i86p2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1i874od</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Meet my friends🌊🏊‍♂️</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i874od</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1i86y7j</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>most compliments i’ve ever gotten on a nail set</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yae7ahr4qree1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1i86smn</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>No filter, just Spanish sun!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lzz0v4yoree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1i85vfe</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Would my nails sell?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i85vfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1i855t6</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Year of the snake nails for cny!!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i855t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1i843x8</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Fastest way of growing your toenails?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93jrcgmd3ree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1i82ga1</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Couple days old but I love</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i82ga1</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1i82ajm</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Why don’t my nails last?!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i82ajm/why_dont_my_nails_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1i805iu</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>about to try russian mani for the first time!</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i805iu/about_to_try_russian_mani_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1i7zhlf</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Retention! When Should I Get a New Set?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7zhlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1i7vk2z</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Damage ?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i7vk2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1i86m4k</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Dip manicure that I did myself</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l50923mmnree1</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1i86hhy</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>DIY Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckprr5mnmree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1i86dxc</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Gel question!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i86dxc/gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1i85izo</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>going to try russian mani for the first time! any tips for pre and post care?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i85izo/going_to_try_russian_mani_for_the_first_time_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1i84hmc</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>ILNP Black Magic</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i84hmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1i8453d</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>How to grow out my nails correctly?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.pinimg.com/originals/de/34/21/de3421ef700135625ffb74b7e6768981.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1i83v60</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Pink blue sparkly nail ✨</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vsg5ca6c1ree1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1i83j2h</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Has anyone used this molds before?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzyrqrucyqee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1i83iec</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Regular polish 👎🏼</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yet849o6yqee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1i839u2</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Engagement Nails!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i839u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1i81qph</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>First set of 2025 ✨</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i81qph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1i81krm</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Appreciation post to these glitter nails.</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2mqtzsmeqee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1i808aa</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Sharp nails, normal?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i808aa/sharp_nails_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1i8qb6t</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Eye of the Storm is truly so stunning</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8qb6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1i8pu52</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>First gel-x</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ndqtycu5wee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1i8pluh</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>My first Manicure.😌</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td9ja33y2wee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1i8otub</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>First try at velvet nails 😊</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mm0dakltvee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1i8oljg</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>my love for a england knows no bounds</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8oljg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1i8ocur</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>they're heeeeeeeere!!!!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8ocur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1i8nk0d</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Fluid Nail Art Attempt #2</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8nk0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1i8ngic</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Pink Magnetic Polish</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8ngic/pink_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1i8nb56</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Identify this polish?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8neuortcdvee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1i8n8g8</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Pink with light blue chrome</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv6q0s3lcvee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1i8mzk3</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Can you recommend a jelly sandwich from this collection?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://deathvalleynails.com/collections/the-valentines-collection?srsltid=AfmBOop8Sz-NGI9ylaMZcan0G-QdbcLpOy-OQIHvI8WEaz4HljVKiyoE</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1i8mqny</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>My birthday ILNP order arrived! Featuring: the magnet!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8mqny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1i8mpqz</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Soulmate on fair skin</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8mmkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1i8lwn7</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>My modest collection as a college student, mostly thanks to Marshall’s lol</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/MyAHpqm.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1i8lwly</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Mysterious Uranus 🪐✨</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8lwly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1i8ltl9</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>It’s giving…Limited Too 🤔</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8ltl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1i8lqy3</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>All the shimmer!!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8lqy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1i8k6uj</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Polish Magnet</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8k6uj/polish_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1i8jxev</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Would you rather pay $15 for 15ml or $10 for 10-12ml?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8jxev/would_you_rather_pay_15_for_15ml_or_10_for_1012ml/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1i8j91w</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Anyone use a tool chest with drawers for polish storage?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k9g97grbuee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1i8j5p5</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>10:02 Nails?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8j5p5/1002_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1i8irwt</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8irwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1i8icvj</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Request for comparison of Mooncat Alien Invasion and Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8icvj/request_for_comparison_of_mooncat_alien_invasion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1i8h8fs</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Please help me pick a color for my next mani!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lixs569wutee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1i8g30d</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Facade vs A Most Destructive Melody</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8g30d/facade_vs_a_most_destructive_melody/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1i8ekbg</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Playing with layering</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6ahzhfk79tee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1i8ef8h</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Nail growth question</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8ef8h/nail_growth_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1i8ebpg</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Slick-adelics🌈💖</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ybq1gfhc8tee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1i8d9p6</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Crime of Passion - I 💕 EdM</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io70rq930tee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1i8cxx8</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Red is just not for me</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqb5uta6ysee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1i8clkb</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Is there an indie brand of nail polish that has good strength to it? (Similar to Xtreme Wear)</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8clkb/is_there_an_indie_brand_of_nail_polish_that_has/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1i8bjqu</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>RIP ring finger nail; you never stood a chance</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42moj96rnsee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1i8band</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Is there a polish that looks like this on its own?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8band</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1i8asax</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Actually shocked this 1.5 year old thermal is still shifting 🍓💖</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8asax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1i8akpf</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>My nails inspired by Phosphophyllite from Land of the Lustrous</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8akpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1i8aa8x</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Nails match our burst pipe 💀</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8aa8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1i8a7e8</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>SAGEBRUSH 🌿</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8a7e8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1i8a4zq</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Mixing UV nail polish with regular</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8a4zq/mixing_uv_nail_polish_with_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1i89wrw</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Inspired by opals set in gold ✨</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i89wrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1i89tv1</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Brand question</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i89tv1/brand_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1i89q1o</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Finally trying almond! Which shape looks best?</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i89q1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1i89ldu</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Cuticle Oil and press-ons?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i89ldu/cuticle_oil_and_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1i89kdf</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Monthly/quarterly boxes. Looking to build a collection</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i89kdf/monthlyquarterly_boxes_looking_to_build_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1i88wzk</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Essie Mademoiselle (pink formula #)</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i88wzk/essie_mademoiselle_pink_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1i88w25</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>an experiment in “nude” (all ILNP)</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i88w25</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1i880s6</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>How often do you paint your toes?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i880s6/how_often_do_you_paint_your_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1i87roe</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Wore this to a Queen cover band concert and was entertained all night!</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nrjvt2f4wree1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1i87rpm</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Help me find a similar polish so I can match my pikmin!</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/515a613awree1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1i877tq</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Good mani polish, bad pedi polish?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i877tq/good_mani_polish_bad_pedi_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1i877od</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Sage🧙🏾‍♀️🪄</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i877od</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1i86szt</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Doom Loop - Breakfast at the End of Time</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i86szt/doom_loop_breakfast_at_the_end_of_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1i86np7</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Blue Swatches</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i86np7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1i85wnx</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>(Purchased) couldn’t wait until Valentine’s Day to wear my new pretties from Arcana Lacquer 😅</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i85wnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1i85u8w</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Curiosity’s Prey</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i85u8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1i85rel</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>What are your favorite thremals?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i85rel/what_are_your_favorite_thremals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1i85466</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Accidentally matched this gorgeous polished nautilus!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yhjfdyxbree1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1i84txs</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Tell me about your favourite ILNP polish!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i84txs/tell_me_about_your_favourite_ilnp_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1i84eec</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Green Eyed Monster</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i84eec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1i84ay0</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Decal first attempt! Constructive comments are welcomed ❤️</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz6tkr615ree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1i83yog</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>The Ultimate It Girl Hot Pink</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i83yog</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1i83m1t</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Some Green Nails</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i83m1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1i83ijo</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Glitter please!</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i83ijo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1i839rr</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Any reccs for shades that look like these pretty screws?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i839rr/any_reccs_for_shades_that_look_like_these_pretty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1i7zkr5</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Pastel pink - like the original Essie Fiji</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i7zkr5/pastel_pink_like_the_original_essie_fiji/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1i8268e</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Sheer nail colour suggestions</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvtvvi49lqee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1i81wc5</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>How to successfully obtain polish from Ulta</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jvitd1diqee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1i80lq7</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>I'm looking for honey shades</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i80lq7/im_looking_for_honey_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1i80h5q</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Feeling witchy</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i80h5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1i8oqvf</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Spring peaches 🍑</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8oqvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1i8o1tp</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>can I still use gel polish for my press ons?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i8o1tp/can_i_still_use_gel_polish_for_my_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1i8mplv</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Fantasy romance</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i8mplv/fantasy_romance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1i8khjd</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Onyx Storm inspired mani</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8khjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1i8je77</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Takumi as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8je77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1i8j5en</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Picnic nails</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8j5en</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1i8io1g</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Finished painting BBNO$ on his practice nail with the new technique and top coat 😭</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ynxo81r6uee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1i8i90i</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>First 22 piece set for Valentines Day 💌</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15nrmea93uee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1i8fn9o</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Gel polishes get sticky and messy.</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i8fn9o/gel_polishes_get_sticky_and_messy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1i8f6f8</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>First time here, a little bit of what I do ✨</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpicts7tetee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1i8eoxd</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Blooming gel</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7amgtx2btee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1i8ebyu</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8ebyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1i886eb</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Sets I've Made This Week (so far...)</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i886eb/sets_ive_made_this_week_so_far/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1i87t62</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Freestyle for Chinese New Year 🧧</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lawcf24kwree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1i870vy</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Thinner Brushes</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i870vy/thinner_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1i86786</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Decal first attempt! Constructive comments are welcomed ❤️</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c9vry8gkree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1i85fz4</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>metal fairy nails for my birthday set.</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuo744sceree1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1i8587z</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Concert nails</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8587z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1i828j0</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Manucure simple sur ongles court ✨</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i828j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1i802r2</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Why do my nails do this?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i802r2/why_do_my_nails_do_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1i8028b</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>I'm so happy :)</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11jg0qyhvpee1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan 25 08:08:54 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_26.xlsx
+++ b/data/collected_data/2025_01_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1098"/>
+  <dimension ref="A1:C1311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19100,6 +19100,3628 @@
         </is>
       </c>
     </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1i9i0w4</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Valentines Nails Round 1</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5iq06sq7h3fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1i9hta1</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Mi primer trabajo blancas negras y stras de
+Manicure</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9hta1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1i9hdyo</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Most recent set.</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9hdyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1i9gn5d</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>What to do?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idz2hxrkz2fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1i9h71r</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Birthday junk(ish) bling nails &amp; toes😍😍</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9h71r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1i9h3rc</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>springtime mani 🌷</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9h3rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1i9gi0w</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>First success</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm0k6azzx2fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1i9g320</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>would you wear these? &lt;3</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9g320</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1i9g0x4</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>A bit messy but it's done after 4 hours</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gn2uilgks2fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1i9ekww</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Which nail shape for my hands?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9ekww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1i9eilq</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>most recent set. these are my natural nails w gel x mani</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo6uu7smc2fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1i9eabv</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>help 🙏</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9eabv/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1i9e3y1</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Just got my nails done. Natural nails with gel polish and gel hardener. I am a chronic nail biter so hardener has helped me grow my nails a little.</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r63b4h2i82fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1i9dsbd</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Gel allergy?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aou1gnza52fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1i9d2r4</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Brown ombré glam set 🤎</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db45e5ohy1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1i9d22n</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Marbled Valentines Set ❣️</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lg7phhay1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1i9cuoa</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>jan 10 vs jan 24</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9cuoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1i9ce9y</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>1st attempt with DIY , Apres GelX Ombré Kit</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwohbqvxr1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1i9c9e6</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Need acrylic advice!!</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9c9e6/need_acrylic_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1i9c0gf</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Thick Nail Glue for Press Ons? (or general press-on advice)</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox0eqseeo1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1i9b756</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Pinterest Inspo</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oayd9j06h1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1i9buuq</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I am obsessed with pressons</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9buuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1i9bsdz</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Help—-what would you do?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8a3gc33cm1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1i9bfga</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Gumball is the shade name. Hard gel fill application.</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4tj9yc5j1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1i9b743</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Need acrylic advice !!!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9b743/need_acrylic_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1i9b2wq</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Dark blue CatEyes</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jae9mkp5g1fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1i9b0o3</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Blooming gel for the winnnn</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpduk2xlf1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1i9asgx</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Blue chrome and silver studs 🥰</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w221pxnd1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1i9aqgn</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Bought some cheap press-ons, filed them down, added gel. Love the way they turned out, edgy and subtle at the same time.</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xa8ndou6d1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1i9a1bk</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Fresh set. I keep wanting red and going basic. But these are SO CUTE</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjivn2r871fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1i99rct</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i99rct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1i98rjz</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>My tech said my nails are HEALTHYY</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipcxykfpw0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1i98d9z</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>tulip garden nails 🌷🌱</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjdw96jkt0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1i980yi</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Manicure question</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i980yi/manicure_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1i97fw5</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>This cut after acrylics, has anyone had this?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v74w8ix8m0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1i97dwm</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Looking for the best nail light (not curing lamp)</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2rp20aul0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1i97df8</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Would you wear these?Apart from length what’s one thing you’d change abt them?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i97df8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1i977sr</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>My first time doing sort of a french nail!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3ijdpqlk0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1i96m09</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>I adore the glittery pink I chose!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5w21uxtf0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1i96gl6</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Butterfly nails</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i96gl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1i96cfm</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>I just got the cutest pink set done for my birthday</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i96cfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1i95t5r</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>I don't pay extra for each color because I make them myself hehe!</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jf7lh9lo90fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1i95ikv</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>🌨️ In January, we wear the ILNP Overcast Collection (minus Daybreak) Glossy vs matte 💙🩶🩵</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i95ikv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1i94qpi</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Is there a way to do acrylics exactly like this? Like, transparent and neon pink? Or does anyone know of a press on brand that looks like this? Other colors would be ok.</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d9i6zth10fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1i94siy</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Drip 💛</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16kjw8lv10fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1i94orl</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>My goth winter nails</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1gwlyk210fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1i94kk6</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>cute lil valentine’s set ❤️</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i94kk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1i94d75</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My Valentine Nails🩷❤️</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vhbhicoyzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1i94ciu</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Growing my nails, how to keep strong</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i94ciu/growing_my_nails_how_to_keep_strong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1i947h8</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>blues? for january? groundbreaking! ❄️🩵</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i947h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1i92rrc</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>acrylic vs gel x at home- which safer/ better overall?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i92rrc/acrylic_vs_gel_x_at_home_which_safer_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1i9412f</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttrooew0wzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1i93qei</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Would yall ask to get this fixed?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i93qei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1i93mt0</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Underside of acrylic nails</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i93mt0/underside_of_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1i936zu</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>I'm starting to make designs</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5j96rzppzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1i934z7</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>What do you think of this design?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tmh0eoapzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1i91w7n</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>new look!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qlqo7sd1gzee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1i91urb</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Why doesn't nail polish stay on my nails?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i91urb/why_doesnt_nail_polish_stay_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1i91uhm</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>valentinesday nails by me!!!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ildip6iofzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1i91q6e</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Should I switch to short square nails?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i91q6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1i91opd</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Anyone have experience with the IBD hard gel?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i91opd/anyone_have_experience_with_the_ibd_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1i9105a</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>The best press ons I’ve ever bought. Just added a layer of builder gel and top coat🤩</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9105a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1i90dzy</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>This Week’s Nails</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i90dzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1i90mu8</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>February Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i90mu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1i90k4q</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>So happy with Holo!</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8j9rhuc6zee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1i8zlcu</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Not done yet but here’s the progress</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8zlcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1i902k4</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>I do my own nails</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i902k4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1i8zwyt</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Should I stick with the almond or go with coffin ?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8zwyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1i8zw0e</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I'm afraid to cut them 😂</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8zw0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1i8zhy0</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Gel polish application</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8zhy0/gel_polish_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1i8za5k</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>First time getting biab [M26]</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlvnvrlxwyee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1i8z9e6</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>£35 down the drain!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8z9e6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1i8z916</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>My manicure on this trip</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkx4tdaiwyee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1i8z0nq</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Acrylics</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azpwol4yuyee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1i8yzgv</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Natural nails turned upwards with builder gel?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8yzgv/natural_nails_turned_upwards_with_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1i8ytk5</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Painting underside of acrylics?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8ytk5/painting_underside_of_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1i8yp0l</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Cute little valentines set ❤️</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8yp0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1i8yn0m</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Most recent set!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hx2d4ei5syee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1i8rzpu</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Removal done wrong?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8rzpu/removal_done_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1i8yi75</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Chrome is chroming</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g07fepi3ryee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1i8utbr</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>What do I really need to buy to do my own press on?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8utbr/what_do_i_really_need_to_buy_to_do_my_own_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1i8v4v8</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Kiss press on 💅</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to0kw5ibzxee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1i8y4b0</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>How do I get an ombre effect?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8y4b0/how_do_i_get_an_ombre_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1i8y1f1</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>New color for the weekend 💜</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8y1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1i8wj6m</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Loving the glitter ✨️</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bkghxglbyee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1i8wqs9</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Made flower nails for my girlfriend - Bonus spooky nail at the end.</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8wqs9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1i8wl3y</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Nails I did for a friend in December</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snr5hcz1cyee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1i8winn</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>A first for my nail tech. I think they did great!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqfd9zqgbyee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1i8wbkq</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Design today 😍</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11wu4bys9yee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1i8vpn7</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Conversation Heart Nails!!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8vpn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1i8vp2f</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Got these done a few days ago, I washed dishes then it bubble and some of it peeled off would it be reasonable to ask for a redo?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g2qtube4yee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1i8v3s4</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Excessive cuticle cutting</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i8v3s4/excessive_cuticle_cutting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1i8uctx</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Bridal nails??</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whmz4rovrxee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1i8u6ua</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>I love my nailtech</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4ii6ab5qxee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1i8t8dh</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Latest experiment</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spf3uug8fxee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1i8seff</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Wicked Checks 🩷💚</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8seff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1i8roou</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>3rd attempt doing my own gel nails!!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdeb0vk5vwee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1i8riod</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>my favorite colors</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8riod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1i8r9fn</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>🖤🤍 Did these yesterday, wdyt</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrzonuicpwee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1i9hcac</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Good UV Lamp</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9hcac/good_uv_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1i9gppa</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>I can't stop staring</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9gppa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1i9gfqh</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Please recommend the most opaque THERMAL nail polish!</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9gfqh/please_recommend_the_most_opaque_thermal_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1i9g2sp</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Holo Taco “Matte Taco” vs. Mooncat “Matte Made in Hell”</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9g2sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1i9fkc4</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Ilnp fun with my kiddo</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g23j6fnn2fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1i9eqf2</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Not bad for a week</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9eqf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1i9enpq</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Triple J’s Hottest 100 inspired!</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9enpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1i9dd3o</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>[Update] Sally Hansen Insta-Dri Syrup Jellies</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9dd3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1i9dc7b</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Ninja polish? Has anyone ever heard of them?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9dc7b/ninja_polish_has_anyone_ever_heard_of_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1i9dalx</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Please tell me clionadh will live up to the hype</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9dalx/please_tell_me_clionadh_will_live_up_to_the_hype/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1i9cled</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Peachy Pink</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9cled/peachy_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1i9ce59</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Nail Swatch Stick Question</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9ce59/nail_swatch_stick_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1i9cc45</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Hydropower by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9cc45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1i9bvif</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Dazzle Dry question.</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9bvif/dazzle_dry_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1i9brm7</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>These shifts are insane 😭</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kzolo6x4m1fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1i9ac4a</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>a definite high moment in my search for the perfect blue 🫐</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9ac4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1i9a8ry</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>What is your favorite nail polish/ nail combos for Lunar New Year? Does anyone know of Lunar New Year collections?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9a8ry/what_is_your_favorite_nail_polish_nail_combos_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1i99p60</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>ILNP Lightwave, with a horseshoe magnet</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fkplkje41fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1i99m13</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Some sparkles in the Snow</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i99m13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1i99bom</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>NCLA for natty nails?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmbpkcj811fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1i996ii</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>My application sucks. Roxy doesn’t care</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i996ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1i98mgm</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Stark white polish on shorties keeps you humble</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i98mgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1i98fnt</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>How do they make it so thick and gel-like?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i98fnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1i98cb3</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Dupe for sally hansen chrome nail makeup?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3x88m9ct0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1i98c13</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Is there an app or off the shelf database that you recommend to track your polishes?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i98c13/is_there_an_app_or_off_the_shelf_database_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1i98166</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>What is this ?</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rvjhluvq0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1i97vep</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>I inherited these old nail polish from my grandma some years ago, anybody knows what brand it could be?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i97vep</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1i97ebp</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Jen &amp; Berries Arrived!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i97ebp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1i975qd</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>ILNP Sugar Plum ✨</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yw12xgq5k0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1i9736g</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>My first is finally here!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09zz23zlj0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1i970rh</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Gallon of Acetone Tips?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i970rh/gallon_of_acetone_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1i96sd0</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Velvetized SHIMMER</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj5eoqo9h0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1i96q4x</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>My modest but mighty collection, swatched!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i96q4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1i96ia4</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Help with vacation mani!</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i96ia4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1i963b9</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Flower/Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkk7x8nub0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1i95q9e</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Singularity</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn1utbc290fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1i95i17</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Mix and match</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hlmnsptf60fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1i95g3m</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>🌨️ In January, we wear the ILNP Overcast Collection (minus Daybreak). Glossy vs matte 💙🩶🩵</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i95g3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1i95eaf</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Two tone distressed</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ownuqgci60fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1i9574v</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Mooncat: After the Rain</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfbfgqgw40fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1i954vp</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>GOAT Dishwasher gloves?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i954vp/goat_dishwasher_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1i952uh</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Recommendations for a topper with heart-shaped glitter?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i952uh/recommendations_for_a_topper_with_heartshaped/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1i950ah</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>I stopped biting my nails a few months ago and I'm wondering how to help these heal or if they are just dead</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i950ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1i94yfu</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Mooncat's Mercury's tears for the win</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i94yfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1i94tem</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Glow in the dark goodness from Mooncat</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i94tem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1i94s6j</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>baby's first skittle...</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i94s6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1i94lcp</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Got bored mid-wear added accent nails a few days in</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y8mn9dc00fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1i94c0m</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Has anyone ordered from Forget Me Not Lacquer before?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i94c0m/has_anyone_ordered_from_forget_me_not_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1i941b5</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>♥️🔥</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i941b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1i93xiu</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>i love this peachy combo ✨</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i93xiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1i93xid</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>January Garnets ❤️✨</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i93xid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1i93vzc</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>ILNP Amped</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i93vzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1i93ot0</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>absolutely in love with this polish! 🧡❤️🚀 DVN Pearls on Mars</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i93ot0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1i93ld5</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>mermaid bait + moonfairy 🤍✨</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i93ld5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1i93kf0</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Dupe for Cirque’s coronation?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7j7fw90kszee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1i93ip1</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Kitty claws in the wild</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k43zyin5szee1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1i9336l</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Swatch request: Coronation + Fairy Dust? 💜🧡🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9336l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1i9308d</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>What do you do when a nail snaps?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uedqozcozee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1i92tf0</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Silly little DIY star stickers</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3ts151xmzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1i92gwy</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>I’m depressed, recommend some shades for me!</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i92gwy/im_depressed_recommend_some_shades_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1i92aw9</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Rainbow Geometric skittle nails</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i92aw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1i91zk7</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Recommendation: long distance relationship to increase nail storage</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4fmp4bqgzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1i91z2u</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Lemons to Lemonade</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i91z2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1i91lkf</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Oh Bees Knees Apparition is BEAUTIFUL 😍</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i91lkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1i91lg2</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>I don’t hate this one as much as I thought I would</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i91lg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1i91jnr</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>HT “Teal With It” vs. ILNP “Funhouse”</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ibzj8ydfdzee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1i91gzn</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Choco Choco Chip</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnb3ygr0dzee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1i91ay3</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Gotta stop buying</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i91ay3/gotta_stop_buying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1i914kt</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Drown My Demons</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i914kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1i90u72</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>What polish with this dress?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i90u72</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1i90t8t</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>ILNP - Seaglass Vs Mooncat - HoH</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vt1v5dz68zee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1i90rll</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Failed my no-buy 😢advice?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i90rll/failed_my_nobuy_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1i90i91</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>February Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i90i91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1i90i1s</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>i love the detail that the elemental sets give link nail polish</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8z4av</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1i908ec</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>First magnetic!</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i908ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1i8zwd1</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>This might be the shiniest nail polish I own 🤍</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoqfxgpk1zee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1i8zh46</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Londontown Vendetta, ILNP Keepsake</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8zh46</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1i8yghu</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Phoenix Nichibotsu (PPU)</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8yghu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1i8ycvu</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>I finally have clear visibility of my whole nail polish collection 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8ycvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1i8y9mt</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Does this clash with my skin tone? Various lighting shown.</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8y9mt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1i8y2rg</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>A Good Day to Make a Cracked Order</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8y2rg/a_good_day_to_make_a_cracked_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1i8wwpi</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Finally received my first LynBD order</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8wwpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1i8wv2y</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>january nails 👾</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7cwwatbeyee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1i8wg5l</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>ILNP Darkest Hour</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5rwbsovayee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1i8n43y</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>💅 beautiful!!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0blxhwbdbvee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1i8w4jw</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Scum &amp; Villainy just perfectly represents my feelings atm. It's also a S.T.U.N.N.E.R!!!!!!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5aesyvq28yee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1i8vvv0</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Got these done a few days ago, I washed dishes then it bubble and some of it peeled off would it be reasonable to ask for a redo?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8vvv0/got_these_done_a_few_days_ago_i_washed_dishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1i8vho6</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Magnetic day 💜🖤</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x71dz4k2yee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1i8v2o0</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Maelstrom vs How Noble</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8v2o0/maelstrom_vs_how_noble/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1i8uzr4</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Pink flakie topper?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i8uzr4/pink_flakie_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1i8u56a</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Anyone have any experience with magnets like these?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bx607ysmpxee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1i8rc9y</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>another Wicked manicure on accident💖💚</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8rc9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1i8r20l</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>My 10 plus year of collecting and moving cross leaves me with this ❤️</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywlb11rfmwee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1i9huux</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Simpsons nails</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9huux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1i9h0ll</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>spring nails</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9h0ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1i9ffkw</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Rosy bouquet 💐</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9ffkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1i9fbbj</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Is this glitter enough to do all ten nails in full coverage?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65quzozxk2fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1i9d5ig</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Valentines</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i9d5ig/valentines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1i9d1e0</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Brown Ombré Glam Set 🤎</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k9y1p34y1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1i9d0pl</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Another Valentines Set💖</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9ghpuqxx1fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1i9b10b</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>I need some advice on how to do my nails in less time!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i9b10b/i_need_some_advice_on_how_to_do_my_nails_in_less/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1i9ays5</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Cute cybercore nails🧚</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9ays5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1i98i71</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Princess Valentine Nails with Polygel</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4iiw41ou0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1i98h1p</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Rawr - it means I love dinosaur nails in dinosaur</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8rv8hjeu0fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1i98chd</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Did me and my sisters nails, let me know what you think!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i98chd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1i97gg2</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Another one for the Disney fans ❤️✨</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i97gg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1i96keh</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Something about a Red Mani… Valentines Day Hot Red Glow and Black Line Art</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i96keh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1i94t27</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>First nail set any tips?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc5l17lz10fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1i93002</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Still practicing doing my own nails (polish work is a solid 6/10)</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i93002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1i90nmb</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>More Horror Nails</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i90nmb/more_horror_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1i8u76y</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>I need advice! Beginner nail artist here</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcapw7y8qxee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1i8py6q</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Would you get teeth on your nails? 🦷</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bht8t7b7wee1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1i8r4ak</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Holo hearts</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8r4ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1i8qpea</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>lunar new year set :)</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i8qpea</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan 26 08:08:58 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_26.xlsx
+++ b/data/collected_data/2025_01_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1311"/>
+  <dimension ref="A1:C1500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22722,6 +22722,3219 @@
         </is>
       </c>
     </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1ia1er7</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Reviews on glowmania Dior ?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ds33zg8g8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ia5y6r</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>nails for my stepdaughters birthday ✨</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia5y6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ia8ot2</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>gold on her fingertips</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j6403j41kafe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ia79kn</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4ich67f2afe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ia7630</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>I never realized nails grow so fast.</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ia7630/i_never_realized_nails_grow_so_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ia3q9i</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Inspired Set</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hh7nnlm19fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1i9xole</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Valentine’s Day inspired from Etsy by BACRYLIX vs how my tech tweaked it for me</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9xole</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ia1n9o</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Do these nails look okay? First time doing press on nails</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kclay1pbi8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ia3bh3</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>What happened?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3i5c8vpx8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ia4da4</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>What would cause this to make a persons nails and finger tips burn like they’ve been dipped in acid?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jf2wtxyr79fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ia52aw</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Dipped and round has changed me forever</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsvdtt4qe9fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ia5hk6</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Critique my nail file shaping - trying to get it almond shaped but looks off…</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnnagrz3j9fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1ia5gf7</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>This is such an amazing set my nail tech made ART lol</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia5gf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1ia5aip</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Ready for February 💖</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfy6m362h9fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1ia4xri</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Who new bugs could look so cute on nails</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rua8ncabd9fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1ia4np5</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>press ons - what are your favorite brands and where do you order them ?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ia4np5/press_ons_what_are_your_favorite_brands_and_where/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ia4dom</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Sweetie Nail Supply Sale?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ia4dom/sweetie_nail_supply_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ia49re</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Pokemon Fun</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzo51xaw69fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ia444z</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Have you been to a junior nail tech?</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ia444z/have_you_been_to_a_junior_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ia32t8</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>❤️‍🔥🖤 new set day</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8ti5j0fv8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1ia2zjk</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Lilac baby boomer with aurora powder</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n387bawku8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1ia2rkh</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Matching nails with my 11 year old. OPI Press Ons continue to impress me.</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/msk94cxhs8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1ia2eli</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>First elaborate nail design, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhjp19z5p8fe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1ia2brr</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>I got chrome nails for the first time and I love them!</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia2brr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1ia2ahp</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>First time using builder gel</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu5eg7y4o8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1ia2a2f</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>clean &lt;3</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia2a2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1ia28nf</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>First time ever doing my own nails (gel x)</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia28nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1ia26i4</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>alice in wonderland nails</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apt46dr5n8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1ia25zj</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Gel-X Help</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia25zj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1ia21p1</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>how do we feel about these?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rubtiqeyl8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1ia1wbw</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Vintage Peacock Nails</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ia1wbw/vintage_peacock_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1ia1vxx</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>☺️ fresh set</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3ljzqwik8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1ia1si2</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Color change up</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia1si2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1ia1r0y</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Purple chrome nails 💅</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hygut6g8j8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1i9yljp</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>My New Haul- Pressons</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9yljp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1i9z09a</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Obsessed w/ my Jan nails</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9koga0awv7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1i9zcc0</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Can someone explain builder gel to me like I’m 5?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9zcc0/can_someone_explain_builder_gel_to_me_like_im_5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1ia1509</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Hey guys, I have a trip upcoming and I really want to do this black lace design on my nails and toes. What would be the easiest way to get this design on them??</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owui2guvd8fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1ia12oi</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Question for the girlies who make press ons</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ia12oi/question_for_the_girlies_who_make_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1ia0t9g</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>First time not doing my own nails in 4 years. also match my everyday makeup &amp; glasses 💕</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia0t9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ia0jwa</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>SATURDAY 💅🏼 ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfefsyau88fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1ia0h1p</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Best Temporary Nails?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ia0h1p/best_temporary_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1ia0b8t</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>In love 🩷</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia0b8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1i9zoek</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Valentine nails</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9zoek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1i9zdio</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Which shape suits me?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx31922xy7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1i9z954</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>🌸 Jelly pink 🌸</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9z954</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1i9z809</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>I think my manicurist is perfect</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqt2u9tix7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1i9yxnv</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Valentine’s Set</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9yxnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1i9yv57</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Gel press-ons are delightful!</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9yv57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1i9xwz3</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>First time trying chrome</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z8tb0r1n7fe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1i9xncm</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Best way to cover up a bruised nail?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9xncm/best_way_to_cover_up_a_bruised_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1i9wow1</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Valentines Themed Nails</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e7htjhbd7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1i9wn3d</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>My passing exam nails</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wn3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1i9vzh9</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Is sculpting gel ok with an acrylate allergy?</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9vzh9/is_sculpting_gel_ok_with_an_acrylate_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1i9wkf3</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Do you think it turned out well? This is the result, I think I became a fan of this technique 😅</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wkf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1i9wcyb</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Beetles reaction</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezsr2i3pa7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1i9upmg</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Looking for full cover tips that go up to a width of 22mm</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9upmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1i9vt8k</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Pink Red ❤️ 🩷 💌</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rd28w5dc67fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1i9vj9r</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>First at home extension set</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9vj9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1i9vfn8</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>3hrs for a soak off, fresh dip and hand painted french. How did I do?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j43pl6bd37fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1i9vdue</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>My first set</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpc902cz27fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1i9v483</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>chinese new yr nails</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9v483</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1i9uhjl</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>GelX Update!</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9uhjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1i9ubvr</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>help pick my nail shape!</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w86pb9dsu6fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1i9tf26</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Trying charms application</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93ydqa6sn6fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1i9tdz8</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Quick pedi</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9tdz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1i9t9aq</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Chrome Obsession!</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yigk1a2km6fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1i9t8gx</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>SHEIN uv gloves ?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9t8gx/shein_uv_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1i9t6nr</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Does this colour suit my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jktnucdyl6fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1i9t49k</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Glue not coming off press ons?</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9t49k/glue_not_coming_off_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1i9t4ip</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Red nails. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9t4ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1i9swef</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Happy with my chrome nails!</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9swef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1i9rkab</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Should I get a fill now or wait a week?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iufame0g96fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1i9q3oc</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Tips on how to improve retention?</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9q3oc/tips_on_how_to_improve_retention/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1i9s2bj</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>recovering my natural nails, it's time to think about me</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xasw9f6d6fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1i9s0d7</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Filming nail videos tips</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9s0d7/filming_nail_videos_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1i9l1af</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Pink nails!</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9l1af</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1i9ryqa</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Do you like chrome finish?</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9ryqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1i9rmkt</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9rmkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1i9rlnp</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Forever in the stars</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9rlnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1i9rgvu</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>What kind of pedicure to clean darkened calluses?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9rgvu/what_kind_of_pedicure_to_clean_darkened_calluses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1i9r69x</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Update from yesterdays clunky nails</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9r69x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1i9r29j</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>got my V Day set!</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9r29j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1i9r0pi</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>OPI Kyoto Pearl Nail Lacquer - Please help me make this stuff dry</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9r0pi/opi_kyoto_pearl_nail_lacquer_please_help_me_make/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1i9qql2</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>My 3-D Crocodile Polka-Dot  5 XL Stiletto nails 🩷🧡</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9qql2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1i9qprc</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>How to make my nails look masculine?</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iesotm3w26fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1i9qczi</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Gel-X vs Builder Gel - which is better/easier for @home?</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i9qczi/gelx_vs_builder_gel_which_is_bettereasier_for_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1i9q8vy</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>New set😁</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thyni8s7z5fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1i9q2n9</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Nails lifting after being in gloves</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9q2n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1i9pt2q</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Just had them done</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oicgxobtv5fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1i9p666</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Tmw not even your hands are photogenic XD</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i8sjv0mq5fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1i9nhc5</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Pretty in Pink</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9nhc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1i9lc79</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>I though I got regular glitter gel polish, but it turned out to be reflective and I love it</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9lc79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1i9kz81</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>New to press-ons, what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sa7ga8jek4fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1i9keee</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>this delicate manicure describes me</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klfjhnqvc4fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1i9kazh</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>One week with these press ons! Clapping for the longest retention I’ve ever had ❤️</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6hwj2mrb4fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1i9jxay</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Sassy Saints Honest Review</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fwkv46r64fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1i9ikid</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>How in the world do I do these??</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9h2c4geo3fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1ia8gm6</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Olive Grove is my That Girl</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia8gm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ia82yv</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Waltz of the flowers by Clionadh dupe?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ia82yv/waltz_of_the_flowers_by_clionadh_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1ia82vi</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>BKL I'm Fast Very Fast Advice</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ia82vi/bkl_im_fast_very_fast_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1ia80os</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>trying the glass nails trend</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6ak1kezfbafe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1ia7in7</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Nail clips for polish removal?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ia7in7/nail_clips_for_polish_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ia7b3i</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Dupes: HT Teal With It (limited edition) and ILNP Funhouse</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43hawbcx2afe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ia7amt</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>inadvertently matched my nails to my shark movie…</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia7amt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ia7a4x</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Drugstore jelly/crellies</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ia7a4x/drugstore_jellycrellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ia6tw8</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Today I learned a valuable lesson about magnetizing while applying top coat.</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/21af4twex9fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ia672w</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>How can I make this with non-gel polish??</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia672w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ia5nvx</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Not mad, just disappointed</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia5nvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1ia5glf</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Essie Petal pushers</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia5glf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1ia4wq3</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Psilocybin</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia4wq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1ia4sv7</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Fun Combo - LynB Designs and Mooncat</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia4sv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1ia4dv4</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Had to run the stairs to get these to transition!</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfb5p62x79fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1ia4dfl</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>hot pink shimmer for less than $2</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia4dfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1ia493t</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Anyone else get antsy after doing a holiday mani?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/s/lztAtcU75v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1ia47ne</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Dupes for Superchic Lacquer?</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atk6urkb69fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1ia3d02</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>so difficult to capture how beautiful Wolfsbane is in person 😩</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia3d02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1ia1d14</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>How to create a custom gel color?</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ia1d14/how_to_create_a_custom_gel_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1ia0mrm</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Comparison of polishes with blue/green shimmer in purple/berry/red base</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia0mrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1ia0jos</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Growing my confidence</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlhu0bvs88fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1ia0ih4</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>"Are they acrylic?"</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia0ih4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1ia0e6x</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Lunar New Year 🐍</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia0e6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1ia0e3r</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Painted Polish Reflective Glitter</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia0e3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1ia0c5w</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>First time trying jelly polish.</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia0c5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1ia03on</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Sparkly baby shower nails 💅🏼👼🏼</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia03on</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1ia02pt</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>When did Essie replace their brushes? Bought brand new bottle and found skinny brush</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ia02pt/when_did_essie_replace_their_brushes_bought_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1i9zp3r</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>First manicure I’m proud of😌</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9zp3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1i9zagf</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Birthday week nails!</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt7br966y7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1i9z1zo</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>What gel base coat can I use to strengthen my nails and keep them from consistently breaking</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9z1zo/what_gel_base_coat_can_i_use_to_strengthen_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1i9y6aq</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>thermonuclear 🔥</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/puqdtrl4p7fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1i9y3br</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>QDTC and clean up brushes, or what order am I supposed to do this in?</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9y3br/qdtc_and_clean_up_brushes_or_what_order_am_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1i9xql5</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>calcifer nails with calcifer 🧡</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9xql5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1i9xclv</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Check Again</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9xclv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1i9xayg</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>After lots and lots of gel, my poor nails have basically given up lol. Im using nailtiques formula 2 + with olive and june cuticle oil, and the blue cross one. I tried nail envy, WAY too many bubbles and it refused to dry. Any recommendations for nail growth?  :(</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9xayg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1i9wvab</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Fashion vs Utility</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wvab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1i9wu39</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>A few comparisons ive been curious about and finally got to make 🥳</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wu39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1i9wsef</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Fairy Dust topper skittle</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wsef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1i9wod4</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>11 days but still strong</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zd45p37d7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1i9wmoo</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer Not Tonight</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wmoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1i9wiyc</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>midnight green shimmer</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wiyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1i9wbch</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>california love</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wbch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1i9w4du</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Well, I know it’s not just black 😂🖤</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10xfld4s87fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1i9vyox</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>How bout that bloodflow?</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9vyox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1i9vtho</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Smoky, hazy, foggy favorites?</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9vtho/smoky_hazy_foggy_favorites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1i9vkoq</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>When you let your cat pick your nail color 🤩 🌈</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/japr987h47fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1i9vfi6</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>My First PPU Polish - Gilded Secrets by Ahmya</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f567t5o437fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1i9v2jq</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Mooncat Freshly Bitten + HoloTaco Linear Holo topper accent nail</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro2s8keh07fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1i9v1a6</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Thanks for influencing me</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9wgtkv707fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1i9uvy1</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>The red-orange-pink I’ve been waiting for 🥹😍</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9uvy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1i9uf8v</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>A comparison no one asked for</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9uf8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1i9u5i4</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>L.A. Colors Vampy🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9u5i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1i9u3kf</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Merkitten ft Natural Nail length 🩷💕💖💞💓💗💝💘</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9u3kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1i9tvhf</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>gorgeous, photogenic polishes...</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9tvhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1i9swah</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Loving Vampire Chocolate 🧛‍♀️ 🍫</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9swah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1i9pu8o</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Volcanic Valentine Skittle Mani!</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9pu8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1i9sehd</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Suggestions for products to restore damaged nails.</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9sehd/suggestions_for_products_to_restore_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1i9sduf</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Last two hauls, first EdM purchase 💕</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge1dn5frf6fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1i9rw84</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Lighting was too good to not take a quick video of the mani</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jj7fejuyb6fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1i9rs79</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>I get the GLL hype now!</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9rs79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1i9rgdf</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>🌊🦈Kevin the Shark🦈🌊</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9rgdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1i9r9vt</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ng72y4r276fe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1i9r148</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Obsessed with ILNP Flicker</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frttlnje56fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1i9qpht</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>American dupe for Hebe Nail Polish remover?</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9qpht/american_dupe_for_hebe_nail_polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1i9qmip</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Mixing my half filled polishes to get new colours!</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fx3l0fmy16fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1i9p7e7</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Crustacean/Cephalopod Themed Polishes?</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9p7e7/crustaceancephalopod_themed_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1i9o4xc</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>TFW You Finally Remember to Use a Topper</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u7iy67ph5fe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1i9o30o</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>New Sub!</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9o30o/new_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1i9nbxw</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Fillable cuticle oil pens?</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i9nbxw/fillable_cuticle_oil_pens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1i9lbxl</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>First clionadh haul!!!</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9lbxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1i9ku9p</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Loving the sparkles</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpzx7vvoi4fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1i9izme</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>🍒How to take photos by yourself? (Angles/ posing/ lighting)</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugw4jr93u3fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1ia7n0z</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Love the look of chrome over cat eye, so I did a different chrome French! Just started doing my own press ons and I'm pretty happy with these!</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d2ep391r6afe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1ia6odi</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Sweet butter and flowers ⚘️</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia6odi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1ia6jf4</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8bnmtw7u9fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1ia5bl2</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Cutie valentine’s nails</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia5bl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1ia4zml</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Who knew bugs could look cute on nails!?</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26jm6sdud9fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1ia3n95</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Under the Sea set</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia3n95</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1ia2vjq</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>🍒 🍸</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ia2vjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1i9zcfv</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>First time french tips</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u92u96sny7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1i9z3q9</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Fresh set! Did them myself!</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/661c7cxow7fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1i9wo9w</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>My first nail art</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9wo9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1i9vxjq</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>3hrs for a soak off, fresh dip and painted french. Feedback please</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c861bew977fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1i9tbit</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Quick pedi</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9tbit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1i9s61n</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>What yall know about that 2013 nail art tho 💅😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icc8wxo2e6fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1i9prip</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>charm heaven</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9prip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1i9pc77</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>I made an 11 year old girl very happy for her birthday</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bbpxbhzr5fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1i9ol4y</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Tip on how to make this heart design?</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i9ol4y/tip_on_how_to_make_this_heart_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1i9o62a</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Some mystical nails 🦎</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ml799nmyh5fe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1i9ntek</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>My dark valentine</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i9ntek</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>